<commit_message>
update module code in makefile and update acs sheets
</commit_message>
<xml_diff>
--- a/src/patterns/acs5_variable_sheets/agexnum_disabilities_poverty.xlsx
+++ b/src/patterns/acs5_variable_sheets/agexnum_disabilities_poverty.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rwalls\gh\srpdio\src\patterns\acs5_variable_sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rwalls/gh/srpdio/src/patterns/acs5_variable_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CC5F3B-5096-40C9-BDB1-8F9B955076CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517E683B-8F81-A64E-AAD0-6E31447470AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27150" yWindow="1695" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{FEA26EBD-3762-0C43-B317-DA7196A35EE9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19200" activeTab="1" xr2:uid="{FEA26EBD-3762-0C43-B317-DA7196A35EE9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Age by number of disabilities" sheetId="1" r:id="rId1"/>
-    <sheet name="Age by disability by poverty" sheetId="2" r:id="rId2"/>
-    <sheet name="Age EJS" sheetId="3" r:id="rId3"/>
+    <sheet name="Age by num disabilities - done" sheetId="1" r:id="rId1"/>
+    <sheet name="Age x disabil x poverty - done" sheetId="2" r:id="rId2"/>
+    <sheet name="Age EJS - done" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -849,10 +849,10 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C15" sqref="C15:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.33203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="25.33203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.33203125" style="4" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" style="4" customWidth="1"/>
@@ -869,7 +869,7 @@
     <col min="13" max="16384" width="25.33203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31">
+    <row r="1" spans="1:13" ht="34">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -906,7 +906,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:13" ht="26">
+    <row r="2" spans="1:13" ht="29">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -938,7 +938,7 @@
       </c>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:13" ht="26">
+    <row r="3" spans="1:13" ht="29">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -972,7 +972,7 @@
       </c>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:13" ht="31">
+    <row r="4" spans="1:13" ht="43">
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
@@ -1008,7 +1008,7 @@
       </c>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:13" ht="46.5">
+    <row r="5" spans="1:13" ht="51">
       <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
@@ -1044,7 +1044,7 @@
       </c>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:13" ht="26">
+    <row r="6" spans="1:13" ht="29">
       <c r="A6" s="5" t="s">
         <v>26</v>
       </c>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:13" ht="26">
+    <row r="7" spans="1:13" ht="29">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:13" ht="31">
+    <row r="8" spans="1:13" ht="43">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:13" ht="46.5">
+    <row r="9" spans="1:13" ht="51">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -1186,7 +1186,7 @@
       </c>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:13" ht="26">
+    <row r="10" spans="1:13" ht="29">
       <c r="A10" s="5" t="s">
         <v>36</v>
       </c>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:13" ht="26">
+    <row r="11" spans="1:13" ht="29">
       <c r="A11" s="5" t="s">
         <v>38</v>
       </c>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:13" ht="31">
+    <row r="12" spans="1:13" ht="43">
       <c r="A12" s="5" t="s">
         <v>41</v>
       </c>
@@ -1292,7 +1292,7 @@
       </c>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:13" ht="46.5">
+    <row r="13" spans="1:13" ht="51">
       <c r="A13" s="5" t="s">
         <v>43</v>
       </c>
@@ -1328,7 +1328,7 @@
       </c>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:13" ht="26">
+    <row r="14" spans="1:13" ht="29">
       <c r="A14" s="5" t="s">
         <v>45</v>
       </c>
@@ -14944,11 +14944,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DAC1550-EDF9-BA42-8BE7-533504D0CD5D}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="24.5" customWidth="1"/>
@@ -14957,7 +14957,7 @@
     <col min="13" max="13" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" ht="46.5">
+    <row r="1" spans="1:13" s="4" customFormat="1" ht="51">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14998,7 +14998,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="9" customFormat="1" ht="38.5">
+    <row r="2" spans="1:13" s="9" customFormat="1" ht="43">
       <c r="A2" s="8" t="s">
         <v>47</v>
       </c>
@@ -15033,7 +15033,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="38.5">
+    <row r="3" spans="1:13" ht="43">
       <c r="A3" s="5" t="s">
         <v>49</v>
       </c>
@@ -15070,7 +15070,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="62">
+    <row r="4" spans="1:13" ht="68">
       <c r="A4" s="5" t="s">
         <v>50</v>
       </c>
@@ -15109,7 +15109,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="62">
+    <row r="5" spans="1:13" ht="71">
       <c r="A5" s="5" t="s">
         <v>53</v>
       </c>
@@ -15150,7 +15150,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="62">
+    <row r="6" spans="1:13" ht="71">
       <c r="A6" s="5" t="s">
         <v>56</v>
       </c>
@@ -15191,7 +15191,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="38.5">
+    <row r="7" spans="1:13" ht="43">
       <c r="A7" s="5" t="s">
         <v>59</v>
       </c>
@@ -15230,7 +15230,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="51">
+    <row r="8" spans="1:13" ht="57">
       <c r="A8" s="5" t="s">
         <v>60</v>
       </c>
@@ -15271,7 +15271,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="51">
+    <row r="9" spans="1:13" ht="57">
       <c r="A9" s="5" t="s">
         <v>62</v>
       </c>
@@ -15312,7 +15312,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="38.5">
+    <row r="10" spans="1:13" ht="43">
       <c r="A10" s="5" t="s">
         <v>64</v>
       </c>
@@ -15349,7 +15349,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="62">
+    <row r="11" spans="1:13" ht="68">
       <c r="A11" s="5" t="s">
         <v>65</v>
       </c>
@@ -15388,7 +15388,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="62">
+    <row r="12" spans="1:13" ht="71">
       <c r="A12" s="5" t="s">
         <v>67</v>
       </c>
@@ -15429,7 +15429,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="62">
+    <row r="13" spans="1:13" ht="71">
       <c r="A13" s="5" t="s">
         <v>69</v>
       </c>
@@ -15470,7 +15470,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="38.5">
+    <row r="14" spans="1:13" ht="43">
       <c r="A14" s="5" t="s">
         <v>71</v>
       </c>
@@ -15509,7 +15509,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="51">
+    <row r="15" spans="1:13" ht="57">
       <c r="A15" s="5" t="s">
         <v>72</v>
       </c>
@@ -15550,7 +15550,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="51">
+    <row r="16" spans="1:13" ht="57">
       <c r="A16" s="5" t="s">
         <v>74</v>
       </c>
@@ -15591,7 +15591,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="38.5">
+    <row r="17" spans="1:13" ht="43">
       <c r="A17" s="5" t="s">
         <v>76</v>
       </c>
@@ -15628,7 +15628,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="62">
+    <row r="18" spans="1:13" ht="68">
       <c r="A18" s="5" t="s">
         <v>77</v>
       </c>
@@ -15667,7 +15667,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="62">
+    <row r="19" spans="1:13" ht="68">
       <c r="A19" s="5" t="s">
         <v>79</v>
       </c>
@@ -15708,7 +15708,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="62">
+    <row r="20" spans="1:13" ht="68">
       <c r="A20" s="5" t="s">
         <v>81</v>
       </c>
@@ -15749,7 +15749,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="38.5">
+    <row r="21" spans="1:13" ht="43">
       <c r="A21" s="5" t="s">
         <v>83</v>
       </c>
@@ -15788,7 +15788,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="51">
+    <row r="22" spans="1:13" ht="57">
       <c r="A22" s="5" t="s">
         <v>84</v>
       </c>
@@ -15829,7 +15829,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="51">
+    <row r="23" spans="1:13" ht="57">
       <c r="A23" s="5" t="s">
         <v>86</v>
       </c>
@@ -15894,16 +15894,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5D2B758-35A9-41BF-B455-0B386702980B}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="5" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" thickBot="1">
+    <row r="1" spans="1:5" ht="18" thickBot="1">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -15920,7 +15920,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="37.5" thickBot="1">
+    <row r="2" spans="1:5" ht="41" thickBot="1">
       <c r="A2" s="12" t="s">
         <v>101</v>
       </c>
@@ -15937,7 +15937,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19" thickBot="1">
+    <row r="3" spans="1:5" ht="21" thickBot="1">
       <c r="A3" s="12" t="s">
         <v>105</v>
       </c>
@@ -15954,7 +15954,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="19" thickBot="1">
+    <row r="4" spans="1:5" ht="21" thickBot="1">
       <c r="A4" s="12" t="s">
         <v>108</v>
       </c>
@@ -15971,7 +15971,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19" thickBot="1">
+    <row r="5" spans="1:5" ht="21" thickBot="1">
       <c r="A5" s="12" t="s">
         <v>112</v>
       </c>
@@ -15988,7 +15988,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="19" thickBot="1">
+    <row r="6" spans="1:5" ht="21" thickBot="1">
       <c r="A6" s="12" t="s">
         <v>115</v>
       </c>

</xml_diff>